<commit_message>
Added proper extract files
</commit_message>
<xml_diff>
--- a/_apidocs/sam-entity-extracts-api/v1/SAM Master Extract Mapping v6.0 FOUO File V2 Layout.xlsx
+++ b/_apidocs/sam-entity-extracts-api/v1/SAM Master Extract Mapping v6.0 FOUO File V2 Layout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelVILLAVICENCIO\Desktop\INT050 New Spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C4057A-CAE0-4128-9B68-8DC8EAA00AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C523C8A-6BCA-4B15-8856-1F4C8DA0FC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2878" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="876">
   <si>
     <t>Breakdown of the string and example below:</t>
   </si>
@@ -2698,6 +2698,9 @@
   </si>
   <si>
     <t>ULTIMATE PARENT UNIQUE ENTITY ID</t>
+  </si>
+  <si>
+    <t>Last Updated: 2022-04-01</t>
   </si>
 </sst>
 </file>
@@ -4286,13 +4289,13 @@
   <sheetPr codeName="Sheet2">
     <tabColor indexed="18"/>
   </sheetPr>
-  <dimension ref="A1:O338"/>
+  <dimension ref="A1:O340"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="N194" sqref="N194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6536,15 +6539,15 @@
         <v>428</v>
       </c>
       <c r="K54" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L54" s="25">
         <f t="shared" ref="L54:L85" si="14">IF(K54="Public",1,IF(K54="FOUO",2,IF(K54="Sensitive",3,IF(K54="System-Only",4))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M54" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N54" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6579,15 +6582,15 @@
         <v>462</v>
       </c>
       <c r="K55" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L55" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M55" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N55" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6622,15 +6625,15 @@
         <v>425</v>
       </c>
       <c r="K56" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L56" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M56" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N56" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6665,15 +6668,15 @@
         <v>426</v>
       </c>
       <c r="K57" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L57" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M57" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N57" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6708,15 +6711,15 @@
         <v>427</v>
       </c>
       <c r="K58" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L58" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M58" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N58" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6751,15 +6754,15 @@
         <v>210</v>
       </c>
       <c r="K59" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L59" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N59" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6794,15 +6797,15 @@
         <v>429</v>
       </c>
       <c r="K60" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L60" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M60" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N60" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6839,15 +6842,15 @@
         <v>494</v>
       </c>
       <c r="K61" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L61" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M61" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N61" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6882,15 +6885,15 @@
         <v>476</v>
       </c>
       <c r="K62" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L62" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M62" s="84" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N62" s="87" t="str">
         <f t="shared" si="3"/>
@@ -6925,15 +6928,15 @@
         <v>467</v>
       </c>
       <c r="K63" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L63" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M63" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N63" s="86" t="str">
         <f t="shared" si="3"/>
@@ -6970,15 +6973,15 @@
         <v>489</v>
       </c>
       <c r="K64" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L64" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M64" s="21" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N64" s="86" t="str">
         <f t="shared" si="3"/>
@@ -7232,15 +7235,15 @@
         <v>428</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L70" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M70" s="21" t="str">
         <f t="shared" ref="M70:M133" si="15">IF(L70&lt;=1,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N70" s="86" t="str">
         <f t="shared" ref="N70:N133" si="16">IF(L70&lt;=2,"X","")</f>
@@ -7275,15 +7278,15 @@
         <v>462</v>
       </c>
       <c r="K71" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L71" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M71" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N71" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7318,15 +7321,15 @@
         <v>425</v>
       </c>
       <c r="K72" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L72" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M72" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N72" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7361,15 +7364,15 @@
         <v>426</v>
       </c>
       <c r="K73" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L73" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M73" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N73" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7404,15 +7407,15 @@
         <v>427</v>
       </c>
       <c r="K74" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L74" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M74" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N74" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7447,15 +7450,15 @@
         <v>210</v>
       </c>
       <c r="K75" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L75" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M75" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N75" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7490,15 +7493,15 @@
         <v>429</v>
       </c>
       <c r="K76" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L76" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M76" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N76" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7535,15 +7538,15 @@
         <v>494</v>
       </c>
       <c r="K77" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L77" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M77" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N77" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7578,15 +7581,15 @@
         <v>476</v>
       </c>
       <c r="K78" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L78" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M78" s="84" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N78" s="87" t="str">
         <f t="shared" si="16"/>
@@ -7621,15 +7624,15 @@
         <v>467</v>
       </c>
       <c r="K79" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L79" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M79" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N79" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7666,15 +7669,15 @@
         <v>489</v>
       </c>
       <c r="K80" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L80" s="25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M80" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N80" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7928,15 +7931,15 @@
         <v>428</v>
       </c>
       <c r="K86" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L86" s="25">
         <f t="shared" ref="L86:L117" si="17">IF(K86="Public",1,IF(K86="FOUO",2,IF(K86="Sensitive",3,IF(K86="System-Only",4))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M86" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N86" s="86" t="str">
         <f t="shared" si="16"/>
@@ -7971,15 +7974,15 @@
         <v>462</v>
       </c>
       <c r="K87" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L87" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M87" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N87" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8014,15 +8017,15 @@
         <v>425</v>
       </c>
       <c r="K88" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L88" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M88" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N88" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8057,15 +8060,15 @@
         <v>426</v>
       </c>
       <c r="K89" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L89" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M89" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N89" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8100,15 +8103,15 @@
         <v>427</v>
       </c>
       <c r="K90" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L90" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M90" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N90" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8143,15 +8146,15 @@
         <v>210</v>
       </c>
       <c r="K91" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L91" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M91" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N91" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8186,15 +8189,15 @@
         <v>429</v>
       </c>
       <c r="K92" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L92" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M92" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N92" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8231,15 +8234,15 @@
         <v>494</v>
       </c>
       <c r="K93" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L93" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M93" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N93" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8274,15 +8277,15 @@
         <v>476</v>
       </c>
       <c r="K94" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L94" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M94" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N94" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8317,15 +8320,15 @@
         <v>467</v>
       </c>
       <c r="K95" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L95" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M95" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N95" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8362,15 +8365,15 @@
         <v>489</v>
       </c>
       <c r="K96" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L96" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M96" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N96" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8624,15 +8627,15 @@
         <v>428</v>
       </c>
       <c r="K102" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L102" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M102" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N102" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8667,15 +8670,15 @@
         <v>462</v>
       </c>
       <c r="K103" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L103" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M103" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N103" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8710,15 +8713,15 @@
         <v>425</v>
       </c>
       <c r="K104" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L104" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M104" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N104" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8753,15 +8756,15 @@
         <v>426</v>
       </c>
       <c r="K105" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L105" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M105" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N105" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8796,15 +8799,15 @@
         <v>427</v>
       </c>
       <c r="K106" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L106" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M106" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N106" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8839,15 +8842,15 @@
         <v>210</v>
       </c>
       <c r="K107" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L107" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M107" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N107" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8882,15 +8885,15 @@
         <v>429</v>
       </c>
       <c r="K108" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L108" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M108" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N108" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8927,15 +8930,15 @@
         <v>494</v>
       </c>
       <c r="K109" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L109" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M109" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N109" s="86" t="str">
         <f t="shared" si="16"/>
@@ -8970,15 +8973,15 @@
         <v>476</v>
       </c>
       <c r="K110" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L110" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M110" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N110" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9013,15 +9016,15 @@
         <v>467</v>
       </c>
       <c r="K111" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L111" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M111" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N111" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9058,15 +9061,15 @@
         <v>489</v>
       </c>
       <c r="K112" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L112" s="25">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M112" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N112" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9320,15 +9323,15 @@
         <v>428</v>
       </c>
       <c r="K118" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L118" s="25">
         <f t="shared" ref="L118:L149" si="18">IF(K118="Public",1,IF(K118="FOUO",2,IF(K118="Sensitive",3,IF(K118="System-Only",4))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M118" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N118" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9363,15 +9366,15 @@
         <v>462</v>
       </c>
       <c r="K119" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L119" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M119" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N119" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9406,15 +9409,15 @@
         <v>425</v>
       </c>
       <c r="K120" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L120" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M120" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N120" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9449,15 +9452,15 @@
         <v>426</v>
       </c>
       <c r="K121" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L121" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M121" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N121" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9492,15 +9495,15 @@
         <v>427</v>
       </c>
       <c r="K122" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L122" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M122" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N122" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9535,15 +9538,15 @@
         <v>210</v>
       </c>
       <c r="K123" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L123" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M123" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N123" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9578,15 +9581,15 @@
         <v>429</v>
       </c>
       <c r="K124" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L124" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M124" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N124" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9623,15 +9626,15 @@
         <v>494</v>
       </c>
       <c r="K125" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L125" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M125" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N125" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9666,15 +9669,15 @@
         <v>476</v>
       </c>
       <c r="K126" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L126" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M126" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N126" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9709,15 +9712,15 @@
         <v>467</v>
       </c>
       <c r="K127" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L127" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M127" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N127" s="86" t="str">
         <f t="shared" si="16"/>
@@ -9754,15 +9757,15 @@
         <v>489</v>
       </c>
       <c r="K128" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L128" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M128" s="21" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N128" s="86" t="str">
         <f t="shared" si="16"/>
@@ -10016,15 +10019,15 @@
         <v>428</v>
       </c>
       <c r="K134" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L134" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M134" s="21" t="str">
         <f t="shared" ref="M134:M209" si="19">IF(L134&lt;=1,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N134" s="86" t="str">
         <f t="shared" ref="N134:N209" si="20">IF(L134&lt;=2,"X","")</f>
@@ -10059,15 +10062,15 @@
         <v>462</v>
       </c>
       <c r="K135" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L135" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M135" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N135" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10102,15 +10105,15 @@
         <v>425</v>
       </c>
       <c r="K136" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L136" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M136" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N136" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10145,15 +10148,15 @@
         <v>426</v>
       </c>
       <c r="K137" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L137" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M137" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N137" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10188,15 +10191,15 @@
         <v>427</v>
       </c>
       <c r="K138" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L138" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M138" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N138" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10231,15 +10234,15 @@
         <v>210</v>
       </c>
       <c r="K139" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L139" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M139" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N139" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10274,15 +10277,15 @@
         <v>429</v>
       </c>
       <c r="K140" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L140" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M140" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N140" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10319,15 +10322,15 @@
         <v>494</v>
       </c>
       <c r="K141" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L141" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M141" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N141" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10362,15 +10365,15 @@
         <v>476</v>
       </c>
       <c r="K142" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L142" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M142" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N142" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10405,15 +10408,15 @@
         <v>467</v>
       </c>
       <c r="K143" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L143" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M143" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N143" s="86" t="str">
         <f t="shared" si="20"/>
@@ -10450,15 +10453,15 @@
         <v>489</v>
       </c>
       <c r="K144" s="26" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L144" s="25">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M144" s="21" t="str">
         <f t="shared" si="19"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N144" s="86" t="str">
         <f t="shared" si="20"/>
@@ -12734,10 +12737,7 @@
         <f t="shared" ref="N196" si="35">IF(L196&lt;=2,"X","")</f>
         <v>X</v>
       </c>
-      <c r="O196" s="137" t="str">
-        <f t="shared" ref="O196" si="36">IF(L196&lt;=3,"X","")</f>
-        <v>X</v>
-      </c>
+      <c r="O196" s="137"/>
     </row>
     <row r="197" spans="1:15" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A197" s="130" t="s">
@@ -13171,19 +13171,19 @@
         <v>398</v>
       </c>
       <c r="L206" s="133">
-        <f t="shared" ref="L206" si="37">IF(K206="Public",1,IF(K206="FOUO",2,IF(K206="Sensitive",3,IF(K206="System-Only",4))))</f>
+        <f t="shared" ref="L206" si="36">IF(K206="Public",1,IF(K206="FOUO",2,IF(K206="Sensitive",3,IF(K206="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M206" s="136" t="str">
-        <f t="shared" ref="M206" si="38">IF(L206&lt;=1,"X","")</f>
+        <f t="shared" ref="M206" si="37">IF(L206&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N206" s="136" t="str">
-        <f t="shared" ref="N206" si="39">IF(L206&lt;=2,"X","")</f>
+        <f t="shared" ref="N206" si="38">IF(L206&lt;=2,"X","")</f>
         <v>X</v>
       </c>
       <c r="O206" s="137" t="str">
-        <f t="shared" ref="O206" si="40">IF(L206&lt;=3,"X","")</f>
+        <f t="shared" ref="O206" si="39">IF(L206&lt;=3,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -13359,11 +13359,11 @@
         <v>2</v>
       </c>
       <c r="M210" s="21" t="str">
-        <f t="shared" ref="M210:M252" si="41">IF(L210&lt;=1,"X","")</f>
+        <f t="shared" ref="M210:M252" si="40">IF(L210&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N210" s="86" t="str">
-        <f t="shared" ref="N210:N252" si="42">IF(L210&lt;=2,"X","")</f>
+        <f t="shared" ref="N210:N252" si="41">IF(L210&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -13404,11 +13404,11 @@
         <v>2</v>
       </c>
       <c r="M211" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N211" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N211" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13449,11 +13449,11 @@
         <v>2</v>
       </c>
       <c r="M212" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N212" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N212" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13494,11 +13494,11 @@
         <v>2</v>
       </c>
       <c r="M213" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N213" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N213" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13538,11 +13538,11 @@
         <v>2</v>
       </c>
       <c r="M214" s="21" t="str">
-        <f t="shared" ref="M214" si="43">IF(L214&lt;=1,"X","")</f>
+        <f t="shared" ref="M214" si="42">IF(L214&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N214" s="86" t="str">
-        <f t="shared" ref="N214" si="44">IF(L214&lt;=2,"X","")</f>
+        <f t="shared" ref="N214" si="43">IF(L214&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -13580,11 +13580,11 @@
         <v>2</v>
       </c>
       <c r="M215" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N215" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N215" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13622,11 +13622,11 @@
         <v>2</v>
       </c>
       <c r="M216" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N216" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N216" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13664,11 +13664,11 @@
         <v>2</v>
       </c>
       <c r="M217" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N217" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N217" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13706,11 +13706,11 @@
         <v>2</v>
       </c>
       <c r="M218" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N218" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N218" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13748,11 +13748,11 @@
         <v>2</v>
       </c>
       <c r="M219" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N219" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N219" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13790,11 +13790,11 @@
         <v>2</v>
       </c>
       <c r="M220" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N220" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N220" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13832,11 +13832,11 @@
         <v>2</v>
       </c>
       <c r="M221" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N221" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N221" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13874,11 +13874,11 @@
         <v>2</v>
       </c>
       <c r="M222" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N222" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N222" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13916,11 +13916,11 @@
         <v>2</v>
       </c>
       <c r="M223" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N223" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N223" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -13958,11 +13958,11 @@
         <v>2</v>
       </c>
       <c r="M224" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N224" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N224" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14000,11 +14000,11 @@
         <v>2</v>
       </c>
       <c r="M225" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N225" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N225" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14042,11 +14042,11 @@
         <v>2</v>
       </c>
       <c r="M226" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N226" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N226" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14084,11 +14084,11 @@
         <v>2</v>
       </c>
       <c r="M227" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N227" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N227" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14126,11 +14126,11 @@
         <v>2</v>
       </c>
       <c r="M228" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N228" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N228" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14168,11 +14168,11 @@
         <v>2</v>
       </c>
       <c r="M229" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N229" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N229" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14210,11 +14210,11 @@
         <v>2</v>
       </c>
       <c r="M230" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N230" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N230" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14249,15 +14249,15 @@
         <v>398</v>
       </c>
       <c r="L231" s="25">
-        <f t="shared" ref="L231:L239" si="45">IF(K231="Public",1,IF(K231="FOUO",2,IF(K231="Sensitive",3,IF(K231="System-Only",4))))</f>
+        <f t="shared" ref="L231:L239" si="44">IF(K231="Public",1,IF(K231="FOUO",2,IF(K231="Sensitive",3,IF(K231="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M231" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N231" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N231" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14292,15 +14292,15 @@
         <v>398</v>
       </c>
       <c r="L232" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M232" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N232" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N232" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14335,15 +14335,15 @@
         <v>398</v>
       </c>
       <c r="L233" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M233" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N233" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N233" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14378,15 +14378,15 @@
         <v>398</v>
       </c>
       <c r="L234" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M234" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N234" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N234" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14423,15 +14423,15 @@
         <v>398</v>
       </c>
       <c r="L235" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M235" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N235" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N235" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14466,15 +14466,15 @@
         <v>398</v>
       </c>
       <c r="L236" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M236" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N236" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N236" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14511,15 +14511,15 @@
         <v>398</v>
       </c>
       <c r="L237" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M237" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N237" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N237" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14554,15 +14554,15 @@
         <v>398</v>
       </c>
       <c r="L238" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M238" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N238" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N238" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14597,15 +14597,15 @@
         <v>398</v>
       </c>
       <c r="L239" s="25">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="M239" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N239" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N239" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14645,11 +14645,11 @@
         <v>2</v>
       </c>
       <c r="M240" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N240" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N240" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14689,11 +14689,11 @@
         <v>2</v>
       </c>
       <c r="M241" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N241" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N241" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14728,15 +14728,15 @@
         <v>398</v>
       </c>
       <c r="L242" s="25">
-        <f t="shared" ref="L242:L266" si="46">IF(K242="Public",1,IF(K242="FOUO",2,IF(K242="Sensitive",3,IF(K242="System-Only",4))))</f>
+        <f t="shared" ref="L242:L266" si="45">IF(K242="Public",1,IF(K242="FOUO",2,IF(K242="Sensitive",3,IF(K242="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M242" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N242" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N242" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14771,15 +14771,15 @@
         <v>398</v>
       </c>
       <c r="L243" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M243" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N243" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N243" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14814,15 +14814,15 @@
         <v>398</v>
       </c>
       <c r="L244" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M244" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N244" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N244" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14857,15 +14857,15 @@
         <v>398</v>
       </c>
       <c r="L245" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M245" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N245" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N245" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14902,15 +14902,15 @@
         <v>398</v>
       </c>
       <c r="L246" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M246" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N246" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N246" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14945,15 +14945,15 @@
         <v>398</v>
       </c>
       <c r="L247" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M247" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N247" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N247" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -14990,15 +14990,15 @@
         <v>398</v>
       </c>
       <c r="L248" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M248" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N248" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N248" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -15033,15 +15033,15 @@
         <v>398</v>
       </c>
       <c r="L249" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M249" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N249" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N249" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -15076,15 +15076,15 @@
         <v>398</v>
       </c>
       <c r="L250" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M250" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N250" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N250" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -15119,15 +15119,15 @@
         <v>398</v>
       </c>
       <c r="L251" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M251" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N251" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N251" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -15162,15 +15162,15 @@
         <v>398</v>
       </c>
       <c r="L252" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M252" s="21" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="N252" s="86" t="str">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="N252" s="86" t="str">
-        <f t="shared" si="42"/>
         <v>X</v>
       </c>
     </row>
@@ -15205,15 +15205,15 @@
         <v>398</v>
       </c>
       <c r="L253" s="25">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="M253" s="21" t="str">
-        <f t="shared" ref="M253:M277" si="47">IF(L253&lt;=1,"X","")</f>
+        <f t="shared" ref="M253:M277" si="46">IF(L253&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N253" s="86" t="str">
-        <f t="shared" ref="N253:N277" si="48">IF(L253&lt;=2,"X","")</f>
+        <f t="shared" ref="N253:N277" si="47">IF(L253&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -15248,15 +15248,15 @@
         <v>398</v>
       </c>
       <c r="L254" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M254" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M254" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N254" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N254" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15291,15 +15291,15 @@
         <v>398</v>
       </c>
       <c r="L255" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M255" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M255" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N255" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N255" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15334,15 +15334,15 @@
         <v>398</v>
       </c>
       <c r="L256" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M256" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M256" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N256" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N256" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15377,15 +15377,15 @@
         <v>398</v>
       </c>
       <c r="L257" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M257" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M257" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N257" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N257" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15422,15 +15422,15 @@
         <v>398</v>
       </c>
       <c r="L258" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M258" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M258" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N258" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N258" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15467,15 +15467,15 @@
         <v>398</v>
       </c>
       <c r="L259" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M259" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M259" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N259" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N259" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15510,15 +15510,15 @@
         <v>398</v>
       </c>
       <c r="L260" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M260" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M260" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N260" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N260" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15555,15 +15555,15 @@
         <v>398</v>
       </c>
       <c r="L261" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M261" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M261" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N261" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N261" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15600,15 +15600,15 @@
         <v>398</v>
       </c>
       <c r="L262" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M262" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M262" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N262" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N262" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15643,15 +15643,15 @@
         <v>398</v>
       </c>
       <c r="L263" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M263" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M263" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N263" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N263" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15688,15 +15688,15 @@
         <v>398</v>
       </c>
       <c r="L264" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M264" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M264" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N264" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N264" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15731,15 +15731,15 @@
         <v>398</v>
       </c>
       <c r="L265" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M265" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M265" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N265" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N265" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15774,15 +15774,15 @@
         <v>398</v>
       </c>
       <c r="L266" s="25">
+        <f t="shared" si="45"/>
+        <v>2</v>
+      </c>
+      <c r="M266" s="21" t="str">
         <f t="shared" si="46"/>
-        <v>2</v>
-      </c>
-      <c r="M266" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N266" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N266" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15821,11 +15821,11 @@
         <v>1</v>
       </c>
       <c r="M267" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N267" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N267" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15867,11 +15867,11 @@
         <v>1</v>
       </c>
       <c r="M268" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N268" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N268" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15913,11 +15913,11 @@
         <v>1</v>
       </c>
       <c r="M269" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N269" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N269" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15955,11 +15955,11 @@
         <v>1</v>
       </c>
       <c r="M270" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N270" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N270" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -15998,11 +15998,11 @@
         <v>1</v>
       </c>
       <c r="M271" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N271" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N271" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16044,11 +16044,11 @@
         <v>1</v>
       </c>
       <c r="M272" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N272" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N272" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16087,11 +16087,11 @@
         <v>2</v>
       </c>
       <c r="M273" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v/>
+      </c>
+      <c r="N273" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N273" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16133,11 +16133,11 @@
         <v>2</v>
       </c>
       <c r="M274" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v/>
+      </c>
+      <c r="N274" s="86" t="str">
         <f t="shared" si="47"/>
-        <v/>
-      </c>
-      <c r="N274" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16179,11 +16179,11 @@
         <v>1</v>
       </c>
       <c r="M275" s="21" t="str">
-        <f t="shared" ref="M275" si="49">IF(L275&lt;=1,"X","")</f>
+        <f t="shared" ref="M275" si="48">IF(L275&lt;=1,"X","")</f>
         <v>X</v>
       </c>
       <c r="N275" s="86" t="str">
-        <f t="shared" ref="N275" si="50">IF(L275&lt;=2,"X","")</f>
+        <f t="shared" ref="N275" si="49">IF(L275&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -16222,11 +16222,11 @@
         <v>1</v>
       </c>
       <c r="M276" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N276" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N276" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16268,11 +16268,11 @@
         <v>1</v>
       </c>
       <c r="M277" s="21" t="str">
+        <f t="shared" si="46"/>
+        <v>X</v>
+      </c>
+      <c r="N277" s="86" t="str">
         <f t="shared" si="47"/>
-        <v>X</v>
-      </c>
-      <c r="N277" s="86" t="str">
-        <f t="shared" si="48"/>
         <v>X</v>
       </c>
     </row>
@@ -16310,11 +16310,11 @@
         <v>2</v>
       </c>
       <c r="M278" s="21" t="str">
-        <f t="shared" ref="M278:M306" si="51">IF(L278&lt;=1,"X","")</f>
+        <f t="shared" ref="M278:M306" si="50">IF(L278&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N278" s="86" t="str">
-        <f t="shared" ref="N278:N306" si="52">IF(L278&lt;=2,"X","")</f>
+        <f t="shared" ref="N278:N306" si="51">IF(L278&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -16356,11 +16356,11 @@
         <v>2</v>
       </c>
       <c r="M279" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N279" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N279" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16398,11 +16398,11 @@
         <v>2</v>
       </c>
       <c r="M280" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N280" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N280" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16442,11 +16442,11 @@
         <v>2</v>
       </c>
       <c r="M281" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N281" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N281" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16486,11 +16486,11 @@
         <v>2</v>
       </c>
       <c r="M282" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N282" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N282" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16530,11 +16530,11 @@
         <v>2</v>
       </c>
       <c r="M283" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N283" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N283" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16574,11 +16574,11 @@
         <v>2</v>
       </c>
       <c r="M284" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N284" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N284" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16618,11 +16618,11 @@
         <v>2</v>
       </c>
       <c r="M285" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N285" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N285" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16657,15 +16657,15 @@
         <v>398</v>
       </c>
       <c r="L286" s="25">
-        <f t="shared" ref="L286:L314" si="53">IF(K286="Public",1,IF(K286="FOUO",2,IF(K286="Sensitive",3,IF(K286="System-Only",4))))</f>
+        <f t="shared" ref="L286:L314" si="52">IF(K286="Public",1,IF(K286="FOUO",2,IF(K286="Sensitive",3,IF(K286="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M286" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N286" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N286" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16700,15 +16700,15 @@
         <v>398</v>
       </c>
       <c r="L287" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M287" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N287" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N287" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16743,15 +16743,15 @@
         <v>398</v>
       </c>
       <c r="L288" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M288" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N288" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N288" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16786,15 +16786,15 @@
         <v>398</v>
       </c>
       <c r="L289" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M289" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N289" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N289" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16829,15 +16829,15 @@
         <v>398</v>
       </c>
       <c r="L290" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M290" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N290" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N290" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16872,15 +16872,15 @@
         <v>398</v>
       </c>
       <c r="L291" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M291" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N291" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N291" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16915,15 +16915,15 @@
         <v>398</v>
       </c>
       <c r="L292" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M292" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N292" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N292" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -16960,15 +16960,15 @@
         <v>398</v>
       </c>
       <c r="L293" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M293" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N293" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N293" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17003,15 +17003,15 @@
         <v>398</v>
       </c>
       <c r="L294" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M294" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N294" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N294" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17046,15 +17046,15 @@
         <v>398</v>
       </c>
       <c r="L295" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M295" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N295" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N295" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17091,15 +17091,15 @@
         <v>398</v>
       </c>
       <c r="L296" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M296" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N296" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N296" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17136,15 +17136,15 @@
         <v>398</v>
       </c>
       <c r="L297" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M297" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N297" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N297" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17179,15 +17179,15 @@
         <v>398</v>
       </c>
       <c r="L298" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M298" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N298" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N298" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17224,15 +17224,15 @@
         <v>398</v>
       </c>
       <c r="L299" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M299" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N299" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N299" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17267,15 +17267,15 @@
         <v>398</v>
       </c>
       <c r="L300" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M300" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N300" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N300" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17310,15 +17310,15 @@
         <v>398</v>
       </c>
       <c r="L301" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M301" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N301" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N301" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17353,15 +17353,15 @@
         <v>398</v>
       </c>
       <c r="L302" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M302" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N302" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N302" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17396,15 +17396,15 @@
         <v>398</v>
       </c>
       <c r="L303" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M303" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N303" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N303" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17439,15 +17439,15 @@
         <v>398</v>
       </c>
       <c r="L304" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M304" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N304" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N304" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17482,15 +17482,15 @@
         <v>398</v>
       </c>
       <c r="L305" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M305" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N305" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N305" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17525,15 +17525,15 @@
         <v>398</v>
       </c>
       <c r="L306" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M306" s="21" t="str">
+        <f t="shared" si="50"/>
+        <v/>
+      </c>
+      <c r="N306" s="86" t="str">
         <f t="shared" si="51"/>
-        <v/>
-      </c>
-      <c r="N306" s="86" t="str">
-        <f t="shared" si="52"/>
         <v>X</v>
       </c>
     </row>
@@ -17568,15 +17568,15 @@
         <v>398</v>
       </c>
       <c r="L307" s="25">
-        <f t="shared" si="53"/>
+        <f t="shared" si="52"/>
         <v>2</v>
       </c>
       <c r="M307" s="21" t="str">
-        <f t="shared" ref="M307:M317" si="54">IF(L307&lt;=1,"X","")</f>
+        <f t="shared" ref="M307:M317" si="53">IF(L307&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N307" s="86" t="str">
-        <f t="shared" ref="N307:N317" si="55">IF(L307&lt;=2,"X","")</f>
+        <f t="shared" ref="N307:N317" si="54">IF(L307&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -17611,15 +17611,15 @@
         <v>398</v>
       </c>
       <c r="L308" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M308" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M308" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N308" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N308" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17656,15 +17656,15 @@
         <v>398</v>
       </c>
       <c r="L309" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M309" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M309" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N309" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N309" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17699,15 +17699,15 @@
         <v>398</v>
       </c>
       <c r="L310" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M310" s="84" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M310" s="84" t="str">
+        <v/>
+      </c>
+      <c r="N310" s="87" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N310" s="87" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17742,15 +17742,15 @@
         <v>398</v>
       </c>
       <c r="L311" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M311" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M311" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N311" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N311" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17787,15 +17787,15 @@
         <v>398</v>
       </c>
       <c r="L312" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M312" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M312" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N312" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N312" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17832,15 +17832,15 @@
         <v>398</v>
       </c>
       <c r="L313" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M313" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M313" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N313" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N313" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17875,15 +17875,15 @@
         <v>398</v>
       </c>
       <c r="L314" s="25">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="M314" s="21" t="str">
         <f t="shared" si="53"/>
-        <v>2</v>
-      </c>
-      <c r="M314" s="21" t="str">
+        <v/>
+      </c>
+      <c r="N314" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N314" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17920,15 +17920,15 @@
         <v>398</v>
       </c>
       <c r="L315" s="25">
-        <f t="shared" ref="L315:L318" si="56">IF(K315="Public",1,IF(K315="FOUO",2,IF(K315="Sensitive",3,IF(K315="System-Only",4))))</f>
+        <f t="shared" ref="L315:L318" si="55">IF(K315="Public",1,IF(K315="FOUO",2,IF(K315="Sensitive",3,IF(K315="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M315" s="21" t="str">
+        <f t="shared" si="53"/>
+        <v/>
+      </c>
+      <c r="N315" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N315" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -17963,15 +17963,15 @@
         <v>398</v>
       </c>
       <c r="L316" s="25">
-        <f t="shared" si="56"/>
+        <f t="shared" si="55"/>
         <v>2</v>
       </c>
       <c r="M316" s="21" t="str">
+        <f t="shared" si="53"/>
+        <v/>
+      </c>
+      <c r="N316" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N316" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -18006,15 +18006,15 @@
         <v>398</v>
       </c>
       <c r="L317" s="25">
-        <f t="shared" si="56"/>
+        <f t="shared" si="55"/>
         <v>2</v>
       </c>
       <c r="M317" s="21" t="str">
+        <f t="shared" si="53"/>
+        <v/>
+      </c>
+      <c r="N317" s="86" t="str">
         <f t="shared" si="54"/>
-        <v/>
-      </c>
-      <c r="N317" s="86" t="str">
-        <f t="shared" si="55"/>
         <v>X</v>
       </c>
     </row>
@@ -18049,21 +18049,21 @@
         <v>403</v>
       </c>
       <c r="L318" s="105">
-        <f t="shared" si="56"/>
+        <f t="shared" si="55"/>
         <v>1</v>
       </c>
       <c r="M318" s="107" t="str">
-        <f t="shared" ref="M318:M338" si="57">IF(L318&lt;=1,"X","")</f>
+        <f t="shared" ref="M318:M338" si="56">IF(L318&lt;=1,"X","")</f>
         <v>X</v>
       </c>
       <c r="N318" s="99" t="str">
-        <f t="shared" ref="N318:N338" si="58">IF(L318&lt;=2,"X","")</f>
+        <f t="shared" ref="N318:N338" si="57">IF(L318&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="319" spans="1:14" ht="25" x14ac:dyDescent="0.35">
       <c r="A319" s="102" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="B319" s="19">
         <v>315</v>
@@ -18084,7 +18084,9 @@
       <c r="H319" s="106" t="s">
         <v>688</v>
       </c>
-      <c r="I319" s="106"/>
+      <c r="I319" s="106" t="s">
+        <v>847</v>
+      </c>
       <c r="J319" s="105" t="s">
         <v>843</v>
       </c>
@@ -18092,21 +18094,21 @@
         <v>398</v>
       </c>
       <c r="L319" s="105">
-        <f t="shared" ref="L319:L336" si="59">IF(K319="Public",1,IF(K319="FOUO",2,IF(K319="Sensitive",3,IF(K319="System-Only",4))))</f>
+        <f t="shared" ref="L319:L336" si="58">IF(K319="Public",1,IF(K319="FOUO",2,IF(K319="Sensitive",3,IF(K319="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M319" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v/>
+      </c>
+      <c r="N319" s="99" t="str">
         <f t="shared" si="57"/>
-        <v/>
-      </c>
-      <c r="N319" s="99" t="str">
-        <f t="shared" si="58"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="320" spans="1:14" ht="25" x14ac:dyDescent="0.35">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A320" s="102" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B320" s="19">
         <v>316</v>
@@ -18128,7 +18130,7 @@
         <v>688</v>
       </c>
       <c r="I320" s="106" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="J320" s="105" t="s">
         <v>843</v>
@@ -18137,21 +18139,21 @@
         <v>398</v>
       </c>
       <c r="L320" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="M320" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v/>
+      </c>
+      <c r="N320" s="99" t="str">
         <f t="shared" si="57"/>
-        <v/>
-      </c>
-      <c r="N320" s="99" t="str">
-        <f t="shared" si="58"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="321" spans="1:14" ht="37.5" x14ac:dyDescent="0.35">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="321" spans="1:14" ht="25" x14ac:dyDescent="0.35">
       <c r="A321" s="102" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B321" s="19">
         <v>317</v>
@@ -18173,7 +18175,7 @@
         <v>688</v>
       </c>
       <c r="I321" s="106" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="J321" s="105" t="s">
         <v>843</v>
@@ -18182,21 +18184,21 @@
         <v>398</v>
       </c>
       <c r="L321" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="M321" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v/>
+      </c>
+      <c r="N321" s="99" t="str">
         <f t="shared" si="57"/>
-        <v/>
-      </c>
-      <c r="N321" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
     <row r="322" spans="1:14" ht="25" x14ac:dyDescent="0.35">
       <c r="A322" s="102" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="B322" s="19">
         <v>318</v>
@@ -18217,9 +18219,7 @@
       <c r="H322" s="106" t="s">
         <v>688</v>
       </c>
-      <c r="I322" s="106" t="s">
-        <v>851</v>
-      </c>
+      <c r="I322" s="106"/>
       <c r="J322" s="105" t="s">
         <v>843</v>
       </c>
@@ -18227,15 +18227,15 @@
         <v>398</v>
       </c>
       <c r="L322" s="105">
-        <f t="shared" si="59"/>
+        <f>IF(K322="Public",1,IF(K322="FOUO",2,IF(K322="Sensitive",3,IF(K322="System-Only",4))))</f>
         <v>2</v>
       </c>
       <c r="M322" s="107" t="str">
-        <f t="shared" si="57"/>
+        <f>IF(L322&lt;=1,"X","")</f>
         <v/>
       </c>
       <c r="N322" s="99" t="str">
-        <f t="shared" si="58"/>
+        <f>IF(L322&lt;=2,"X","")</f>
         <v>X</v>
       </c>
     </row>
@@ -18268,15 +18268,15 @@
         <v>403</v>
       </c>
       <c r="L323" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M323" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N323" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N323" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18309,15 +18309,15 @@
         <v>403</v>
       </c>
       <c r="L324" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M324" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N324" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N324" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18350,15 +18350,15 @@
         <v>403</v>
       </c>
       <c r="L325" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M325" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N325" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N325" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18391,15 +18391,15 @@
         <v>403</v>
       </c>
       <c r="L326" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M326" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N326" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N326" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18432,15 +18432,15 @@
         <v>403</v>
       </c>
       <c r="L327" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M327" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N327" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N327" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18473,15 +18473,15 @@
         <v>403</v>
       </c>
       <c r="L328" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M328" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N328" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N328" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18514,15 +18514,15 @@
         <v>403</v>
       </c>
       <c r="L329" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M329" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N329" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N329" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18555,15 +18555,15 @@
         <v>403</v>
       </c>
       <c r="L330" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M330" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N330" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N330" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18596,15 +18596,15 @@
         <v>403</v>
       </c>
       <c r="L331" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M331" s="107" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N331" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N331" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18637,15 +18637,15 @@
         <v>403</v>
       </c>
       <c r="L332" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M332" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N332" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N332" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18678,15 +18678,15 @@
         <v>403</v>
       </c>
       <c r="L333" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M333" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N333" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N333" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18719,15 +18719,15 @@
         <v>403</v>
       </c>
       <c r="L334" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M334" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N334" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N334" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18760,15 +18760,15 @@
         <v>403</v>
       </c>
       <c r="L335" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M335" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N335" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N335" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18801,15 +18801,15 @@
         <v>403</v>
       </c>
       <c r="L336" s="105">
-        <f t="shared" si="59"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="M336" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N336" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N336" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18842,15 +18842,15 @@
         <v>403</v>
       </c>
       <c r="L337" s="105">
-        <f t="shared" ref="L337" si="60">IF(K337="Public",1,IF(K337="FOUO",2,IF(K337="Sensitive",3,IF(K337="System-Only",4))))</f>
+        <f t="shared" ref="L337" si="59">IF(K337="Public",1,IF(K337="FOUO",2,IF(K337="Sensitive",3,IF(K337="System-Only",4))))</f>
         <v>1</v>
       </c>
       <c r="M337" s="100" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N337" s="99" t="str">
         <f t="shared" si="57"/>
-        <v>X</v>
-      </c>
-      <c r="N337" s="99" t="str">
-        <f t="shared" si="58"/>
         <v>X</v>
       </c>
     </row>
@@ -18888,12 +18888,17 @@
         <v>1</v>
       </c>
       <c r="M338" s="101" t="str">
+        <f t="shared" si="56"/>
+        <v>X</v>
+      </c>
+      <c r="N338" s="101" t="str">
         <f t="shared" si="57"/>
         <v>X</v>
       </c>
-      <c r="N338" s="101" t="str">
-        <f t="shared" si="58"/>
-        <v>X</v>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A340" s="1" t="s">
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -18904,12 +18909,12 @@
     <mergeCell ref="A2:N2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="N321:N337 M332:M337 M338:N338 M5:N5 M176:N176 M184:N185 M8:N174 M197:N205 M207:N331 M187:N195">
+  <conditionalFormatting sqref="N320:N337 M332:M337 M338:N338 M5:N5 M176:N176 M184:N185 M8:N174 M197:N205 M187:N195 M207:N331">
     <cfRule type="expression" dxfId="13" priority="32">
       <formula>(M5="X")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N321:N337 M338:N338 M332:M337 M5:N5 M176:N176 M184:N185 M8:N174 M197:N205 M207:N331 M187:N195">
+  <conditionalFormatting sqref="N320:N337 M338:N338 M332:M337 M5:N5 M176:N176 M184:N185 M8:N174 M197:N205 M187:N195 M207:N331">
     <cfRule type="cellIs" dxfId="12" priority="31" operator="equal">
       <formula>"CSV Only"</formula>
     </cfRule>
@@ -18974,8 +18979,8 @@
       <formula>"CSV Only"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H197:H204 H207:H338 H8:H185 H187:H194" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H197:H204 H8:H185 H187:H194 H207:H338" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>MandatoryOptional</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>